<commit_message>
Committed after adding more actionkeywords like verify element, compare link text by Ravikanth
</commit_message>
<xml_diff>
--- a/KeywordDriven/src/test/java/dataEngine/DataEngine.xlsx
+++ b/KeywordDriven/src/test/java/dataEngine/DataEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="12650" windowWidth="22260" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
+    <workbookView windowHeight="12650" windowWidth="22260" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Test Steps" r:id="rId1" sheetId="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="70">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -127,64 +127,109 @@
     <t>Results</t>
   </si>
   <si>
+    <t>Data Set</t>
+  </si>
+  <si>
+    <t>ravikaanthe@rediffmail.com</t>
+  </si>
+  <si>
+    <t>test@123</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>Menu_Navigation</t>
+  </si>
+  <si>
+    <t>Click on T-SHIRTS main menue</t>
+  </si>
+  <si>
+    <t>btn_Tshirts</t>
+  </si>
+  <si>
+    <t>TS_009</t>
+  </si>
+  <si>
+    <t>compareGetText</t>
+  </si>
+  <si>
+    <t>Compare title of the T-SHIRTS main menue page</t>
+  </si>
+  <si>
+    <t>title_Tshirts</t>
+  </si>
+  <si>
+    <t>T-shirts</t>
+  </si>
+  <si>
+    <t>TS_010</t>
+  </si>
+  <si>
+    <t>Validating Main Menue navigations</t>
+  </si>
+  <si>
+    <t>Close Browser</t>
+  </si>
+  <si>
+    <t>Logout_01</t>
+  </si>
+  <si>
+    <t>TS_011</t>
+  </si>
+  <si>
+    <t>Verify the webelement Username on page</t>
+  </si>
+  <si>
+    <t>Verify the webelement Passwrod on page</t>
+  </si>
+  <si>
+    <t>TS_007</t>
+  </si>
+  <si>
+    <t>TS_012</t>
+  </si>
+  <si>
+    <t>Verify the webelement login button</t>
+  </si>
+  <si>
+    <t>Compare link text of the customer account who has logged-in</t>
+  </si>
+  <si>
+    <t>lnk_custaccount</t>
+  </si>
+  <si>
+    <t>compareLinkText</t>
+  </si>
+  <si>
+    <t>ravi reddy</t>
+  </si>
+  <si>
+    <t>TS_013</t>
+  </si>
+  <si>
+    <t>TS_014</t>
+  </si>
+  <si>
+    <t>verifyElement</t>
+  </si>
+  <si>
+    <t>Verifying the account of user who logged-in</t>
+  </si>
+  <si>
+    <t>TS_015</t>
+  </si>
+  <si>
+    <t>Verify_Account</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>Data Set</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>ravikaanthe@rediffmail.com</t>
-  </si>
-  <si>
-    <t>test@123</t>
-  </si>
-  <si>
-    <t>input</t>
-  </si>
-  <si>
-    <t>Menu_Navigation</t>
-  </si>
-  <si>
-    <t>Click on T-SHIRTS main menue</t>
-  </si>
-  <si>
-    <t>btn_Tshirts</t>
-  </si>
-  <si>
-    <t>TS_009</t>
-  </si>
-  <si>
-    <t>compareGetText</t>
-  </si>
-  <si>
-    <t>Compare title of the T-SHIRTS main menue page</t>
-  </si>
-  <si>
-    <t>title_Tshirts</t>
-  </si>
-  <si>
-    <t>T-shirts</t>
-  </si>
-  <si>
-    <t>TS_010</t>
-  </si>
-  <si>
-    <t>Validating Main Menue navigations</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>Close Browser</t>
-  </si>
-  <si>
-    <t>Logout_01</t>
-  </si>
-  <si>
-    <t>TS_011</t>
   </si>
 </sst>
 </file>
@@ -192,7 +237,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -562,17 +607,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="15.6328125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="41.1796875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="51.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.26953125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="22.453125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="24.90625" collapsed="true"/>
   </cols>
@@ -594,7 +639,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>34</v>
@@ -615,10 +660,10 @@
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>35</v>
+        <v>68</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -636,8 +681,8 @@
         <v>14</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
-        <v>35</v>
+      <c r="G3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -648,19 +693,17 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>35</v>
+        <v>63</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -671,19 +714,19 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -694,17 +737,17 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>35</v>
+        <v>63</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -715,99 +758,206 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="F8" s="5"/>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>48</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F9" s="2"/>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>35</v>
+      <c r="G10" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="E11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
-        <v>35</v>
+      <c r="F16" s="2"/>
+      <c r="G16" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -817,8 +967,8 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F4" xr:uid="{E460A94D-7A09-45AA-8564-D57B4C352F82}"/>
-    <hyperlink r:id="rId2" ref="F5" xr:uid="{BDF14D56-9AFB-41C4-99B0-98EA40E2C18E}"/>
+    <hyperlink r:id="rId1" ref="F5" xr:uid="{E460A94D-7A09-45AA-8564-D57B4C352F82}"/>
+    <hyperlink r:id="rId2" ref="F7" xr:uid="{BDF14D56-9AFB-41C4-99B0-98EA40E2C18E}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -827,10 +977,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713D4E8D-EC36-4313-B503-DE2A5B2115DA}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -864,36 +1014,50 @@
       <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>35</v>
+      <c r="D2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>35</v>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified verify element to highlight object and added log4j.xml file to main project folder
</commit_message>
<xml_diff>
--- a/KeywordDriven/src/test/java/dataEngine/DataEngine.xlsx
+++ b/KeywordDriven/src/test/java/dataEngine/DataEngine.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView windowHeight="12650" windowWidth="22260" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Steps" r:id="rId1" sheetId="1"/>
-    <sheet name="Test Cases" r:id="rId2" sheetId="2"/>
+    <sheet name="Test Steps" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="87">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -223,13 +223,64 @@
     <t>Verify_Account</t>
   </si>
   <si>
+    <t>Verify_MyAccount_Page</t>
+  </si>
+  <si>
+    <t>TS_016</t>
+  </si>
+  <si>
+    <t>TS_017</t>
+  </si>
+  <si>
+    <t>TS_018</t>
+  </si>
+  <si>
+    <t>TS_019</t>
+  </si>
+  <si>
+    <t>TS_020</t>
+  </si>
+  <si>
+    <t>Verify the elements of My Account Page</t>
+  </si>
+  <si>
+    <t>Verify the element btn_OrderHistory of My Account Page</t>
+  </si>
+  <si>
+    <t>Verify the element btn_MycreditSlips of My Account Page</t>
+  </si>
+  <si>
+    <t>Verify the element btn_Myaddress of My Account Page</t>
+  </si>
+  <si>
+    <t>Verify the element btn_Mypersonalinfo of My Account Page</t>
+  </si>
+  <si>
+    <t>Verify the elements btn_Mywhishlist of My Account Page</t>
+  </si>
+  <si>
+    <t>btn_OrderHistory</t>
+  </si>
+  <si>
+    <t>btn_MycreditSlips</t>
+  </si>
+  <si>
+    <t>btn_Myaddress</t>
+  </si>
+  <si>
+    <t>btn_Mypersonalinfo</t>
+  </si>
+  <si>
+    <t>btn_Mywhishlist</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
     <t>FAIL</t>
   </si>
   <si>
     <t>Chrome</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -237,7 +288,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,20 +346,20 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -332,7 +383,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -349,10 +400,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -387,7 +438,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -422,7 +473,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -516,21 +567,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -547,7 +598,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -599,23 +650,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.6328125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.1796875" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="51.90625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="14.26953125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="22.453125" collapsed="true"/>
@@ -660,10 +711,10 @@
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -682,7 +733,7 @@
       </c>
       <c r="F3" s="2"/>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -703,7 +754,7 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -726,7 +777,7 @@
         <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -747,7 +798,7 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -770,7 +821,7 @@
         <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -791,7 +842,7 @@
       </c>
       <c r="F8" s="5"/>
       <c r="G8" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -812,7 +863,7 @@
       </c>
       <c r="F9" s="2"/>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -831,7 +882,7 @@
       </c>
       <c r="F10" s="2"/>
       <c r="G10" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -854,7 +905,7 @@
         <v>60</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -873,119 +924,224 @@
       </c>
       <c r="F12" s="2"/>
       <c r="G12" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>46</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="F14" s="2"/>
       <c r="G14" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="E16" s="2" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" t="s">
-        <v>69</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule dxfId="1" operator="containsText" priority="1" text="FAIL" type="containsText">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F5" xr:uid="{E460A94D-7A09-45AA-8564-D57B4C352F82}"/>
-    <hyperlink r:id="rId2" ref="F7" xr:uid="{BDF14D56-9AFB-41C4-99B0-98EA40E2C18E}"/>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{E460A94D-7A09-45AA-8564-D57B4C352F82}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{BDF14D56-9AFB-41C4-99B0-98EA40E2C18E}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713D4E8D-EC36-4313-B503-DE2A5B2115DA}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713D4E8D-EC36-4313-B503-DE2A5B2115DA}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.6328125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.1796875" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="41.1796875" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="12.6328125" collapsed="true"/>
   </cols>
@@ -1015,7 +1171,7 @@
         <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1029,44 +1185,58 @@
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule dxfId="0" operator="containsText" priority="1" text="FAIL" type="containsText">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commiting to local by adding new verify element lnk_women
</commit_message>
<xml_diff>
--- a/KeywordDriven/src/test/java/dataEngine/DataEngine.xlsx
+++ b/KeywordDriven/src/test/java/dataEngine/DataEngine.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="90">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -274,13 +274,22 @@
     <t>btn_Mywhishlist</t>
   </si>
   <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Verify the elements lnk_Women of My Account Page</t>
+  </si>
+  <si>
+    <t>lnk_Women</t>
+  </si>
+  <si>
+    <t>TS_021</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>Chrome</t>
   </si>
 </sst>
 </file>
@@ -658,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -711,10 +720,10 @@
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -733,7 +742,7 @@
       </c>
       <c r="F3" s="2"/>
       <c r="G3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -754,7 +763,7 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -777,7 +786,7 @@
         <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -798,7 +807,7 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -821,7 +830,7 @@
         <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -842,7 +851,7 @@
       </c>
       <c r="F8" s="5"/>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -863,7 +872,7 @@
       </c>
       <c r="F9" s="2"/>
       <c r="G9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -882,7 +891,7 @@
       </c>
       <c r="F10" s="2"/>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -905,7 +914,7 @@
         <v>60</v>
       </c>
       <c r="G11" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -924,7 +933,7 @@
       </c>
       <c r="F12" s="2"/>
       <c r="G12" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -932,7 +941,7 @@
         <v>67</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>74</v>
@@ -945,7 +954,7 @@
       </c>
       <c r="F13" s="2"/>
       <c r="G13" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -953,7 +962,7 @@
         <v>67</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>75</v>
@@ -966,7 +975,7 @@
       </c>
       <c r="F14" s="2"/>
       <c r="G14" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -974,7 +983,7 @@
         <v>67</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>76</v>
@@ -987,7 +996,7 @@
       </c>
       <c r="F15" s="2"/>
       <c r="G15" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -995,7 +1004,7 @@
         <v>67</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>77</v>
@@ -1008,15 +1017,15 @@
       </c>
       <c r="F16" s="2"/>
       <c r="G16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>78</v>
@@ -1029,91 +1038,112 @@
       </c>
       <c r="F17" s="2"/>
       <c r="G17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>46</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F19" s="2"/>
       <c r="G19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="G20" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="E21" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" t="s">
-        <v>84</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1136,7 +1166,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1171,7 +1201,7 @@
         <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1185,7 +1215,7 @@
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1199,7 +1229,7 @@
         <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -1213,7 +1243,7 @@
         <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -1227,7 +1257,7 @@
         <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing changes to repository by Ravi
</commit_message>
<xml_diff>
--- a/KeywordDriven/src/test/java/dataEngine/DataEngine.xlsx
+++ b/KeywordDriven/src/test/java/dataEngine/DataEngine.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="87">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1011,7 +1011,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>67</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>50</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
Modified, DataEngine to include Verify Element events to verify menu items. Also modified action keywords to highlight verifylinktext element
</commit_message>
<xml_diff>
--- a/KeywordDriven/src/test/java/dataEngine/DataEngine.xlsx
+++ b/KeywordDriven/src/test/java/dataEngine/DataEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Steps" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="82">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -163,9 +163,6 @@
     <t>T-shirts</t>
   </si>
   <si>
-    <t>TS_010</t>
-  </si>
-  <si>
     <t>Validating Main Menue navigations</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
     <t>Logout_01</t>
   </si>
   <si>
-    <t>TS_011</t>
-  </si>
-  <si>
     <t>Verify the webelement Username on page</t>
   </si>
   <si>
@@ -187,9 +181,6 @@
     <t>TS_007</t>
   </si>
   <si>
-    <t>TS_012</t>
-  </si>
-  <si>
     <t>Verify the webelement login button</t>
   </si>
   <si>
@@ -205,42 +196,18 @@
     <t>ravi reddy</t>
   </si>
   <si>
-    <t>TS_013</t>
-  </si>
-  <si>
-    <t>TS_014</t>
-  </si>
-  <si>
     <t>verifyElement</t>
   </si>
   <si>
     <t>Verifying the account of user who logged-in</t>
   </si>
   <si>
-    <t>TS_015</t>
-  </si>
-  <si>
     <t>Verify_Account</t>
   </si>
   <si>
     <t>Verify_MyAccount_Page</t>
   </si>
   <si>
-    <t>TS_016</t>
-  </si>
-  <si>
-    <t>TS_017</t>
-  </si>
-  <si>
-    <t>TS_018</t>
-  </si>
-  <si>
-    <t>TS_019</t>
-  </si>
-  <si>
-    <t>TS_020</t>
-  </si>
-  <si>
     <t>Verify the elements of My Account Page</t>
   </si>
   <si>
@@ -274,13 +241,31 @@
     <t>btn_Mywhishlist</t>
   </si>
   <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Verify the menu element lnk_Women of My Account Page</t>
+  </si>
+  <si>
+    <t>lnk_Women</t>
+  </si>
+  <si>
+    <t>Verify the menu element lnk_Dresses of My Account Page</t>
+  </si>
+  <si>
+    <t>lnk_Dresses</t>
+  </si>
+  <si>
+    <t>Verify the menu element lnk_Tshirts of My Account Page</t>
+  </si>
+  <si>
+    <t>lnk_Tshirts</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>Chrome</t>
   </si>
 </sst>
 </file>
@@ -288,7 +273,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,6 +283,29 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -349,13 +357,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -658,462 +670,525 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.1796875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="51.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.26953125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="22.453125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="24.90625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="21.1796875" collapsed="true"/>
+    <col min="2" max="2" style="6" width="8.7265625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="51.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="6" width="14.26953125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="6" width="22.453125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="6" width="24.90625" collapsed="true"/>
+    <col min="7" max="16384" style="6" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>86</v>
+      <c r="F2" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="7"/>
       <c r="G3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="C8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="D13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="C16" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="C17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="C18" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="C20" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="F21" s="7"/>
+      <c r="G21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="2" t="s">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="F23" s="7"/>
+      <c r="G23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
+      <c r="B24" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" t="s">
-        <v>84</v>
+      <c r="F24" s="7"/>
+      <c r="G24" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1135,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713D4E8D-EC36-4313-B503-DE2A5B2115DA}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1156,7 +1231,7 @@
       <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1171,35 +1246,35 @@
         <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -1207,18 +1282,18 @@
         <v>39</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>33</v>
@@ -1227,7 +1302,7 @@
         <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added code related to mobile browser testing and committing
</commit_message>
<xml_diff>
--- a/KeywordDriven/src/test/java/dataEngine/DataEngine.xlsx
+++ b/KeywordDriven/src/test/java/dataEngine/DataEngine.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="79">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -55,12 +55,6 @@
     <t>Action_Keyword</t>
   </si>
   <si>
-    <t>Navigate to website</t>
-  </si>
-  <si>
-    <t>navigate</t>
-  </si>
-  <si>
     <t>Enter Email Address in Email Address field</t>
   </si>
   <si>
@@ -253,22 +247,16 @@
     <t>lnk_Tshirts</t>
   </si>
   <si>
+    <t>1TS_002</t>
+  </si>
+  <si>
+    <t>Open Browser</t>
+  </si>
+  <si>
+    <t>mopenBrowser</t>
+  </si>
+  <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>1TS_002</t>
-  </si>
-  <si>
-    <t>Open Browser</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>openBrowser</t>
   </si>
 </sst>
 </file>
@@ -681,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -709,16 +697,16 @@
         <v>9</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -726,20 +714,18 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="7" t="s">
         <v>77</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -747,39 +733,37 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="8"/>
+        <v>46</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="E3" s="8" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="F3" s="8"/>
-      <c r="G3" s="7" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="7" t="s">
-        <v>77</v>
+        <v>34</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -787,43 +771,37 @@
         <v>1</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>77</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="7" t="s">
-        <v>77</v>
+        <v>34</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -831,238 +809,203 @@
         <v>1</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>77</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="7" t="s">
-        <v>77</v>
-      </c>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="7" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="8"/>
+        <v>50</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="E10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="7" t="s">
-        <v>77</v>
+        <v>52</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>53</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D11" s="8"/>
       <c r="E11" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>77</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="8"/>
+        <v>59</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="E12" s="8" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="F12" s="8"/>
-      <c r="G12" s="7" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="7" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F14" s="8"/>
-      <c r="G14" s="7" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F15" s="8"/>
-      <c r="G15" s="7" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>70</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F17" s="8"/>
-      <c r="G17" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>71</v>
@@ -1071,19 +1014,16 @@
         <v>72</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F18" s="8"/>
-      <c r="G18" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>73</v>
@@ -1092,117 +1032,81 @@
         <v>74</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F19" s="8"/>
-      <c r="G19" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="F20" s="8"/>
-      <c r="G20" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="8" t="s">
+      <c r="C23" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="D23" s="8"/>
       <c r="E23" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F23" s="8"/>
-      <c r="G23" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="7" t="s">
-        <v>77</v>
-      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
@@ -1211,8 +1115,8 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F5" xr:uid="{E460A94D-7A09-45AA-8564-D57B4C352F82}"/>
-    <hyperlink r:id="rId2" ref="F7" xr:uid="{BDF14D56-9AFB-41C4-99B0-98EA40E2C18E}"/>
+    <hyperlink r:id="rId1" ref="F4" xr:uid="{E460A94D-7A09-45AA-8564-D57B4C352F82}"/>
+    <hyperlink r:id="rId2" ref="F6" xr:uid="{BDF14D56-9AFB-41C4-99B0-98EA40E2C18E}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1224,7 +1128,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1240,13 +1144,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1254,70 +1158,60 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>77</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>77</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>77</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>78</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>77</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">

</xml_diff>

<commit_message>
Committing better stable code with mobile automation using real device
</commit_message>
<xml_diff>
--- a/KeywordDriven/src/test/java/dataEngine/DataEngine.xlsx
+++ b/KeywordDriven/src/test/java/dataEngine/DataEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Steps" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -272,12 +272,6 @@
   </si>
   <si>
     <t>btn_Mywhishlist</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
   <si>
     <t>Chrome</t>
@@ -287,7 +281,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,6 +291,29 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -348,13 +365,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -659,461 +680,403 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="51.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.453125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.1796875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.7265625" style="6"/>
+    <col min="3" max="3" width="51.90625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.26953125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.453125" style="6" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.90625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="8.7265625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F2" s="7" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" t="s">
-        <v>84</v>
-      </c>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" t="s">
-        <v>84</v>
-      </c>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G5" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" t="s">
-        <v>84</v>
-      </c>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G7" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" t="s">
-        <v>84</v>
-      </c>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" t="s">
-        <v>84</v>
-      </c>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" t="s">
-        <v>84</v>
-      </c>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G11" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" t="s">
-        <v>84</v>
-      </c>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" t="s">
-        <v>84</v>
-      </c>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" t="s">
-        <v>84</v>
-      </c>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" t="s">
-        <v>84</v>
-      </c>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
+      <c r="D21" s="7"/>
+      <c r="E21" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" t="s">
-        <v>84</v>
-      </c>
+      <c r="F21" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
@@ -1134,8 +1097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713D4E8D-EC36-4313-B503-DE2A5B2115DA}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1155,7 +1118,7 @@
       <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1169,9 +1132,6 @@
       <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -1183,9 +1143,6 @@
       <c r="C3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D3" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -1197,9 +1154,6 @@
       <c r="C4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -1211,9 +1165,6 @@
       <c r="C5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D5" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -1224,9 +1175,6 @@
       </c>
       <c r="C6" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Successful run of Mobile script and web application script
</commit_message>
<xml_diff>
--- a/KeywordDriven/src/test/java/dataEngine/DataEngine.xlsx
+++ b/KeywordDriven/src/test/java/dataEngine/DataEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Steps" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="86">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -275,13 +275,16 @@
   </si>
   <si>
     <t>Chrome</t>
+  </si>
+  <si>
+    <t>Web Application Testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,6 +331,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -365,17 +383,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -678,405 +699,416 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.1796875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.7265625" style="6"/>
-    <col min="3" max="3" width="51.90625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.26953125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.453125" style="6" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.90625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="8.7265625" style="6"/>
+    <col min="1" max="1" width="21.1796875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.7265625" style="4"/>
+    <col min="3" max="3" width="51.90625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.26953125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.453125" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.90625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F6" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F8" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F12" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E14" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E15" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D17" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E17" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="7" t="s">
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D18" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E18" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D19" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="7" t="s">
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D20" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F20" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="7" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E21" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="7" t="s">
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C22" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7" t="s">
+      <c r="D22" s="5"/>
+      <c r="E22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="7"/>
+      <c r="F22" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
@@ -1085,8 +1117,8 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" xr:uid="{E460A94D-7A09-45AA-8564-D57B4C352F82}"/>
-    <hyperlink ref="F7" r:id="rId2" xr:uid="{BDF14D56-9AFB-41C4-99B0-98EA40E2C18E}"/>
+    <hyperlink ref="F6" r:id="rId1" xr:uid="{E460A94D-7A09-45AA-8564-D57B4C352F82}"/>
+    <hyperlink ref="F8" r:id="rId2" xr:uid="{BDF14D56-9AFB-41C4-99B0-98EA40E2C18E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1097,83 +1129,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713D4E8D-EC36-4313-B503-DE2A5B2115DA}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.6328125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.1796875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.1796875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.6328125" style="10" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="8.7265625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="11" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>